<commit_message>
updated the class as done
</commit_message>
<xml_diff>
--- a/Project3/MetodosESB.xlsx
+++ b/Project3/MetodosESB.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
   <si>
     <t>Filipe</t>
   </si>
@@ -516,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,6 +619,9 @@
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="B10" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="C10" s="2" t="s">
         <v>4</v>
       </c>
@@ -626,6 +629,9 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>24</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>4</v>
@@ -803,7 +809,7 @@
     </row>
     <row r="9" spans="1:4" ht="14.45" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:4" ht="14.45" x14ac:dyDescent="0.3"/>
-    <row r="19" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3"/>
+    <row r="19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added input output to splitter
</commit_message>
<xml_diff>
--- a/Project3/MetodosESB.xlsx
+++ b/Project3/MetodosESB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="19665" windowHeight="8520"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="19665" windowHeight="8520" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="54">
   <si>
     <t>Filipe</t>
   </si>
@@ -166,6 +166,18 @@
   </si>
   <si>
     <t>falta limpar as classes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input da webprobe </t>
+  </si>
+  <si>
+    <t>Split da mensagem em companies esb que são passadas assynconamente para o serviço configurado no esb</t>
+  </si>
+  <si>
+    <t>On Going</t>
+  </si>
+  <si>
+    <t>Mensagem com as companhias partidas</t>
   </si>
 </sst>
 </file>
@@ -522,7 +534,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -764,8 +776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -807,14 +819,29 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>35</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>36</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add: Updated with report tasks
</commit_message>
<xml_diff>
--- a/Project3/MetodosESB.xlsx
+++ b/Project3/MetodosESB.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="19665" windowHeight="8520" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="96" windowWidth="19668" windowHeight="8520"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
     <sheet name="Serviços In Out" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="62">
   <si>
     <t>Filipe</t>
   </si>
@@ -42,12 +41,6 @@
     <t>João</t>
   </si>
   <si>
-    <t>design decisions</t>
-  </si>
-  <si>
-    <t>deploy instructions</t>
-  </si>
-  <si>
     <t>responsibilities (tabela com packages)</t>
   </si>
   <si>
@@ -57,12 +50,6 @@
     <t>EJB / webservice</t>
   </si>
   <si>
-    <t>diagrama dinâmico</t>
-  </si>
-  <si>
-    <t>diagrama estático</t>
-  </si>
-  <si>
     <t>Listar Users</t>
   </si>
   <si>
@@ -178,6 +165,42 @@
   </si>
   <si>
     <t>Mensagem com as companhias partidas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BPM print </t>
+  </si>
+  <si>
+    <t>Design decisions - BPM</t>
+  </si>
+  <si>
+    <t>Design decisions - WS</t>
+  </si>
+  <si>
+    <t>Design decisions - Splitter</t>
+  </si>
+  <si>
+    <t>diagrama dinâmico - BPM</t>
+  </si>
+  <si>
+    <t>diagrama dinâmico - WS+ESB</t>
+  </si>
+  <si>
+    <t>Incluir alguma explicação</t>
+  </si>
+  <si>
+    <t>Only if necessary</t>
+  </si>
+  <si>
+    <t>Deployment instructions - projecto</t>
+  </si>
+  <si>
+    <t>Deployment instructions - jbpm</t>
+  </si>
+  <si>
+    <t>Joao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joao </t>
   </si>
 </sst>
 </file>
@@ -221,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -231,6 +254,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -532,22 +556,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="59.28515625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="59.33203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="29" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="48.140625" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="2"/>
+    <col min="3" max="3" width="16.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="48.109375" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -561,209 +585,260 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="B10" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="B20" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:4" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C27" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>10</v>
+        <v>52</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -776,97 +851,85 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="34.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="48.140625" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="39.5546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="34.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="48.109375" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="3"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="B6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D8" s="3"/>
     </row>
-    <row r="19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>